<commit_message>
before removal of redundant clusterdistance
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimgo\Desktop\Unief\bdap\NearestNeighbour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B967CAC-F041-4577-AF16-D377A1304D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9583F29-CFBA-4353-84B8-E7F98BAFC953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84" yWindow="1536" windowWidth="17268" windowHeight="8964" xr2:uid="{0E9354EC-6FAD-482B-A39C-02D32E233951}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0E9354EC-6FAD-482B-A39C-02D32E233951}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
   <si>
     <t>spambase</t>
   </si>
@@ -52,9 +53,6 @@
     <t>covtype</t>
   </si>
   <si>
-    <t>acc</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
@@ -65,6 +63,81 @@
   </si>
   <si>
     <t>sknn</t>
+  </si>
+  <si>
+    <t>4.49s</t>
+  </si>
+  <si>
+    <t>264.04s</t>
+  </si>
+  <si>
+    <t>1.55s</t>
+  </si>
+  <si>
+    <t>319.06s</t>
+  </si>
+  <si>
+    <t>3.04s</t>
+  </si>
+  <si>
+    <t>1.41s</t>
+  </si>
+  <si>
+    <t>110.40s</t>
+  </si>
+  <si>
+    <t>0.70s</t>
+  </si>
+  <si>
+    <t>0.74s</t>
+  </si>
+  <si>
+    <t>39.82s</t>
+  </si>
+  <si>
+    <t>0.86s</t>
+  </si>
+  <si>
+    <t>0.65s</t>
+  </si>
+  <si>
+    <t>0.24s</t>
+  </si>
+  <si>
+    <t>0.03s</t>
+  </si>
+  <si>
+    <t>0.02s</t>
+  </si>
+  <si>
+    <t>retrieval</t>
+  </si>
+  <si>
+    <t>distance error</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>nclusters</t>
+  </si>
+  <si>
+    <t>npartitions</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>retrieval rate</t>
   </si>
 </sst>
 </file>
@@ -100,8 +173,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,17 +493,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EB0572-3E67-43DE-BC52-0D5335DB0E60}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -438,66 +521,474 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.99</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.99</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.99</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
-        <v>1.47E-2</v>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
-        <v>6.9999999999999999E-4</v>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
       </c>
       <c r="C8">
-        <v>2.7000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="E8">
+        <v>44.13</v>
+      </c>
+      <c r="F8">
+        <v>6.6E-3</v>
+      </c>
+      <c r="G8">
+        <v>0.114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>0.78</v>
+      </c>
+      <c r="D9">
+        <v>0.71</v>
+      </c>
+      <c r="E9">
+        <v>0.92</v>
+      </c>
+      <c r="F9">
+        <v>0.71</v>
+      </c>
+      <c r="G9">
+        <v>0.68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49090AD1-69E1-4840-8C21-9D67D2CAD153}">
+  <dimension ref="C3:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="G11">
+        <v>44.13</v>
+      </c>
+      <c r="H11">
+        <v>6.6E-3</v>
+      </c>
+      <c r="I11">
+        <v>0.114</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <v>0.78</v>
+      </c>
+      <c r="F12">
+        <v>0.71</v>
+      </c>
+      <c r="G12">
+        <v>0.92</v>
+      </c>
+      <c r="H12">
+        <v>0.71</v>
+      </c>
+      <c r="I12">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>63</v>
+      </c>
+      <c r="F13">
+        <v>32</v>
+      </c>
+      <c r="G13">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <v>25</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>256</v>
+      </c>
+      <c r="F14">
+        <v>256</v>
+      </c>
+      <c r="G14">
+        <v>256</v>
+      </c>
+      <c r="H14">
+        <v>256</v>
+      </c>
+      <c r="I14">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>